<commit_message>
Finally commit befor merging
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -854,26 +854,28 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>110364955</t>
+          <t>110412718</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>QA Engineer - SuperApp</t>
+          <t>Junior Python Developer</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-11-08T08:34:19+0300</t>
+          <t>2024-11-08T12:32:14+0300</t>
         </is>
       </c>
       <c r="G10" t="b">
@@ -881,45 +883,39 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110364955</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110412718</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>AndroidStudio, XCode, Git (GitLab). Будет плюсом знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и ООП, request, allure, pytest, json, csv, os, re. Знание Selenium, SeleniumWebDriver...</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Выполнение прогонов тест-кейсов по проекту. Разработка тестовых артефактов: чек-листы, чит-листы, тест-кейсы, планы тестирования. Фиксация и ведения...</t>
-        </is>
-      </c>
+          <t>Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Опыт написания REST приложений на любом &lt;highlighttext&gt;Python&lt;/highlighttext&gt; фреймворке (Flask, FastAPI, Django и др.). Понимание основ SQL и...</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>110412718</t>
+          <t>110412671</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Junior Python Developer</t>
+          <t>Python разработчик</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>65000</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E11" t="n">
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2024-11-08T12:32:14+0300</t>
+          <t>2024-11-08T12:31:57+0300</t>
         </is>
       </c>
       <c r="G11" t="b">
@@ -927,25 +923,29 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110412718</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110412671</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Опыт написания REST приложений на любом &lt;highlighttext&gt;Python&lt;/highlighttext&gt; фреймворке (Flask, FastAPI, Django и др.). Понимание основ SQL и...</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
+          <t>Коммерческий опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; – от 1 года. Хорошее знание Aiohttp. Понимание базовых принципов работы API и опыт взаимодействия с...</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Анализ API-сторонних сервисов и доработка собственных. Реализация stateless микросервисов. Разработка внутренних библиотек. Оптимизация узких мест в основной архитектуре продукта.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>110412671</t>
+          <t>110364955</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Python разработчик</t>
+          <t>QA Engineer - SuperApp</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -959,7 +959,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2024-11-08T12:31:57+0300</t>
+          <t>2024-11-08T08:34:19+0300</t>
         </is>
       </c>
       <c r="G12" t="b">
@@ -967,36 +967,36 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110412671</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110364955</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Коммерческий опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; – от 1 года. Хорошее знание Aiohttp. Понимание базовых принципов работы API и опыт взаимодействия с...</t>
+          <t>AndroidStudio, XCode, Git (GitLab). Будет плюсом знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и ООП, request, allure, pytest, json, csv, os, re. Знание Selenium, SeleniumWebDriver...</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Анализ API-сторонних сервисов и доработка собственных. Реализация stateless микросервисов. Разработка внутренних библиотек. Оптимизация узких мест в основной архитектуре продукта.</t>
+          <t>Выполнение прогонов тест-кейсов по проекту. Разработка тестовых артефактов: чек-листы, чит-листы, тест-кейсы, планы тестирования. Фиксация и ведения...</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>110121148</t>
+          <t>110429201</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Python-разработчик</t>
+          <t>Junior Java Developer</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>130000</v>
+        <v>50000</v>
       </c>
       <c r="D13" t="n">
-        <v>170000</v>
+        <v>70000</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2024-11-05T12:44:48+0300</t>
+          <t>2024-11-08T15:38:31+0300</t>
         </is>
       </c>
       <c r="G13" t="b">
@@ -1013,36 +1013,36 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110121148</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110429201</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; от 2 лет. Опыт работы с библиотеками для обработки PDF, Excel, DWG данных. Навыки работы с...</t>
+          <t xml:space="preserve">Знание основных шаблонов проектирования. Умение читать чужой код. Знание Spring, Hibernate. Опыт программирования на языках PHP, Ruby или &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Ответственность. </t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Разработка Telegram-бота с использованием библиотеки &lt;highlighttext&gt;python&lt;/highlighttext&gt;-telegram-bot. Настройка команд для загрузки и обработки файлов (PDF, Excel, DWG). </t>
+          <t>Разработка нового и поддержка существующего функционала сервиса. Участие в разработке мобильных приложений сервиса.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>110414678</t>
+          <t>110121148</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Middle+ Тестировщик</t>
+          <t>Python-разработчик</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>130000</v>
       </c>
       <c r="D14" t="n">
-        <v>250000</v>
+        <v>170000</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2024-11-08T12:42:32+0300</t>
+          <t>2024-11-05T12:44:48+0300</t>
         </is>
       </c>
       <c r="G14" t="b">
@@ -1059,36 +1059,36 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110414678</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110121148</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Выбирать методы и инструменты тестирования. Есть опыт тестирования Web-приложений и АPI. Хорошо знаешь и понимаешь техники тест-дизайна.</t>
+          <t>Опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; от 2 лет. Опыт работы с библиотеками для обработки PDF, Excel, DWG данных. Навыки работы с...</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Продукт, отвечающий за цифровую бухгалтерию для маркетплейсов. Планировать тестирование. Создавать тестовые случаи и сценарии. Проводить ручное тестирование. Автоматизировать регрессионное тестирование. </t>
+          <t xml:space="preserve">Разработка Telegram-бота с использованием библиотеки &lt;highlighttext&gt;python&lt;/highlighttext&gt;-telegram-bot. Настройка команд для загрузки и обработки файлов (PDF, Excel, DWG). </t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>110429201</t>
+          <t>110324773</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Junior Java Developer</t>
+          <t>ГИС специалист</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>50000</v>
+        <v>117000</v>
       </c>
       <c r="D15" t="n">
-        <v>70000</v>
+        <v>117000</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2024-11-08T15:38:31+0300</t>
+          <t>2024-11-07T14:44:58+0300</t>
         </is>
       </c>
       <c r="G15" t="b">
@@ -1105,17 +1105,17 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110429201</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110324773</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Знание основных шаблонов проектирования. Умение читать чужой код. Знание Spring, Hibernate. Опыт программирования на языках PHP, Ruby или &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Ответственность. </t>
+          <t>...геодезической, землеустроительной нефтегазовой сфере. Знакомы с пространственными базами данных и публикацией сервисов. Имеете опыт составления SQL-запросов и знаете &lt;highlighttext&gt;Python&lt;/highlighttext&gt;).</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Разработка нового и поддержка существующего функционала сервиса. Участие в разработке мобильных приложений сервиса.</t>
+          <t>Работа с массивами данных в ГИС, сопровождение, наполнение и актуализация базы пространственных данных по объектам ПАО «Транснефть». Сбор, обработка, структурирование...</t>
         </is>
       </c>
     </row>
@@ -1168,28 +1168,26 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>110324773</t>
+          <t>110425944</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ГИС специалист</t>
+          <t>Python developer / Python разработчик</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>117000</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>117000</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2024-11-07T14:44:58+0300</t>
+          <t>2024-11-08T15:10:17+0300</t>
         </is>
       </c>
       <c r="G17" t="b">
@@ -1197,29 +1195,29 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110324773</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110425944</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>...геодезической, землеустроительной нефтегазовой сфере. Знакомы с пространственными базами данных и публикацией сервисов. Имеете опыт составления SQL-запросов и знаете &lt;highlighttext&gt;Python&lt;/highlighttext&gt;).</t>
+          <t>Опытом разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;3. Глубокими знаниями и практическим опытом работы с Asyncio. Уверенными знаниями Linux. Умением работать в команде...</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Работа с массивами данных в ГИС, сопровождение, наполнение и актуализация базы пространственных данных по объектам ПАО «Транснефть». Сбор, обработка, структурирование...</t>
+          <t>Разработка и поддержка приложений на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;3 с использованием Asyncio. Оптимизация существующего кода и улучшение производительности приложений. Взаимодействие с командой...</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>110336864</t>
+          <t>110110217</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Middle Python Developer</t>
+          <t>QA engineer</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1233,7 +1231,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2024-11-07T18:16:47+0300</t>
+          <t>2024-11-05T10:57:20+0300</t>
         </is>
       </c>
       <c r="G18" t="b">
@@ -1241,43 +1239,45 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110336864</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110110217</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Опыт разработки 3-х лет в коммерческих проектах с применением веб-сервисов. Отличное знание языка &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Понимание того как делаются...</t>
+          <t>...части совершенствования процессов тестирования. Желание развиваться в автоматизации тест кейсов (Java или &lt;highlighttext&gt;Python&lt;/highlighttext&gt;). Самостоятельность. Опыт автоматизации тест кейсов (Java, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;).</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Разработка веб-сервисов: мобильное API, API для web-приложения (админка), разработка интеграционных и служебных сервисов. Реализация сервисов с использованием потоковой...</t>
+          <t>Выполнять функциональное тестирование веб- и мобильных приложений. Анализировать и тестировать требования. Писать тестовую документацию: чек-листы, тест-планы и тест...</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>110110217</t>
+          <t>110414678</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>QA engineer</t>
+          <t>Middle+ Тестировщик</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
+        <v>250000</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2024-11-05T10:57:20+0300</t>
+          <t>2024-11-08T12:42:32+0300</t>
         </is>
       </c>
       <c r="G19" t="b">
@@ -1285,45 +1285,43 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110110217</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110414678</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>...части совершенствования процессов тестирования. Желание развиваться в автоматизации тест кейсов (Java или &lt;highlighttext&gt;Python&lt;/highlighttext&gt;). Самостоятельность. Опыт автоматизации тест кейсов (Java, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;).</t>
+          <t>Выбирать методы и инструменты тестирования. Есть опыт тестирования Web-приложений и АPI. Хорошо знаешь и понимаешь техники тест-дизайна.</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Выполнять функциональное тестирование веб- и мобильных приложений. Анализировать и тестировать требования. Писать тестовую документацию: чек-листы, тест-планы и тест...</t>
+          <t xml:space="preserve">Продукт, отвечающий за цифровую бухгалтерию для маркетплейсов. Планировать тестирование. Создавать тестовые случаи и сценарии. Проводить ручное тестирование. Автоматизировать регрессионное тестирование. </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>110411464</t>
+          <t>110336864</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Разработчик Django / Python</t>
+          <t>Middle Python Developer</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>700</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2024-11-08T12:25:23+0300</t>
+          <t>2024-11-07T18:16:47+0300</t>
         </is>
       </c>
       <c r="G20" t="b">
@@ -1331,17 +1329,17 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110411464</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110336864</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и Django от 2 лет. Понимание принципов ООП и опыт применения их в реальных проектах. </t>
+          <t>Опыт разработки 3-х лет в коммерческих проектах с применением веб-сервисов. Отличное знание языка &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Понимание того как делаются...</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Разработка и поддержка веб-приложений на Django и &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Участие в проектировании и улучшении архитектуры проектов. Оптимизация производительности и обеспечение...</t>
+          <t>Разработка веб-сервисов: мобильное API, API для web-приложения (админка), разработка интеграционных и служебных сервисов. Реализация сервисов с использованием потоковой...</t>
         </is>
       </c>
     </row>
@@ -1392,12 +1390,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>108794013</t>
+          <t>109756686</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Senior/Middle+ Backend Developer</t>
+          <t>Младший Python разработчик</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1411,7 +1409,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2024-10-17T12:34:13+0300</t>
+          <t>2024-10-31T14:49:55+0300</t>
         </is>
       </c>
       <c r="G22" t="b">
@@ -1419,43 +1417,45 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108794013</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109756686</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Разрабатывали коммерческие приложения не менее 5 лет. Качественно тестируете свой код и свободно работаете с чужим. Разбираетесь в классических алгоритмах...</t>
+          <t>Образование В/НВ в ведущих российских ВУЗах. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и SQL. Хорошие аналитические способности, ориентированность на результат.</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Поддерживали программное обеспечение от написания до выкладки в продакшен. Умеете мониторить работу готового ПО и оперативно реагировать на проблемы. </t>
+          <t xml:space="preserve">Разработка и поддержка веб/десктоп-приложений: разработка функциональности, модулей, компонентов и интерфейсов с использованием различных языков программирования и технологий. </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>110336628</t>
+          <t>110411464</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Инженер-тестировщик</t>
+          <t>Разработчик Django / Python</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
+        <v>700</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2024-11-07T18:04:57+0300</t>
+          <t>2024-11-08T12:25:23+0300</t>
         </is>
       </c>
       <c r="G23" t="b">
@@ -1463,17 +1463,17 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110336628</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110411464</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Понимание процесса тестирования, роли тестировщика в команде, знание теории тестирования. Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Опыт работы с ADB. Знание SQL на...</t>
+          <t xml:space="preserve">Опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и Django от 2 лет. Понимание принципов ООП и опыт применения их в реальных проектах. </t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Фиксация обнаруженных дефектов в баг-трекере (Jira). Верификация и валидация исправленных дефектов. Тест-анализ, работа с аналитикой, техническими и бизнес...</t>
+          <t>Разработка и поддержка веб-приложений на Django и &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Участие в проектировании и улучшении архитектуры проектов. Оптимизация производительности и обеспечение...</t>
         </is>
       </c>
     </row>
@@ -1524,12 +1524,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>109756686</t>
+          <t>108794013</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Младший Python разработчик</t>
+          <t>Senior/Middle+ Backend Developer</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2024-10-31T14:49:55+0300</t>
+          <t>2024-10-17T12:34:13+0300</t>
         </is>
       </c>
       <c r="G25" t="b">
@@ -1551,45 +1551,43 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109756686</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108794013</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Образование В/НВ в ведущих российских ВУЗах. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и SQL. Хорошие аналитические способности, ориентированность на результат.</t>
+          <t>Разрабатывали коммерческие приложения не менее 5 лет. Качественно тестируете свой код и свободно работаете с чужим. Разбираетесь в классических алгоритмах...</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Разработка и поддержка веб/десктоп-приложений: разработка функциональности, модулей, компонентов и интерфейсов с использованием различных языков программирования и технологий. </t>
+          <t xml:space="preserve">Поддерживали программное обеспечение от написания до выкладки в продакшен. Умеете мониторить работу готового ПО и оперативно реагировать на проблемы. </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>110383575</t>
+          <t>110336628</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Стажер (IT и аналитика)</t>
+          <t>Инженер-тестировщик</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>63500</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E26" t="n">
+        <v>0</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2024-11-08T10:08:32+0300</t>
+          <t>2024-11-07T18:04:57+0300</t>
         </is>
       </c>
       <c r="G26" t="b">
@@ -1597,43 +1595,45 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110383575</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110336628</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Высшее образование или студенты последних курсов по специальностям: статистика, математика, экономика, IT. Знание MS Excel. Опыт работы в 1С...</t>
+          <t>Понимание процесса тестирования, роли тестировщика в команде, знание теории тестирования. Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Опыт работы с ADB. Знание SQL на...</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Выполнение функций по документообороту. Выгрузка отчетов в 1С. Полный цикл ведения контрактов с аптечными сетями и производителями. </t>
+          <t>Фиксация обнаруженных дефектов в баг-трекере (Jira). Верификация и валидация исправленных дефектов. Тест-анализ, работа с аналитикой, техническими и бизнес...</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>110286973</t>
+          <t>110383575</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Руководитель IT департамента (CTO/CIO)</t>
+          <t>Стажер (IT и аналитика)</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>63500</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
-      <c r="E27" t="n">
-        <v>0</v>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2024-11-07T09:22:33+0300</t>
+          <t>2024-11-08T10:08:32+0300</t>
         </is>
       </c>
       <c r="G27" t="b">
@@ -1641,45 +1641,43 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110286973</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110383575</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Стек языков: PHP5, PHP7, PHP8, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Perl, Go, JS, Kotlin, Java, C-Object, Swift. Стек серверный технологий...</t>
+          <t>Высшее образование или студенты последних курсов по специальностям: статистика, математика, экономика, IT. Знание MS Excel. Опыт работы в 1С...</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Техническое управление проектами(продуктами) компании, решение возникающих проблем, согласование принимаемых архитектурных решений, разбор инцидентов, оптимизация инфраструктуры. Участие во встречах по...</t>
+          <t xml:space="preserve">Выполнение функций по документообороту. Выгрузка отчетов в 1С. Полный цикл ведения контрактов с аптечными сетями и производителями. </t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>110286826</t>
+          <t>110286973</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Intern Data Analyst / Стажер - аналитик данных</t>
+          <t>Руководитель IT департамента (CTO/CIO)</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E28" t="n">
+        <v>0</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2024-11-07T09:20:15+0300</t>
+          <t>2024-11-07T09:22:33+0300</t>
         </is>
       </c>
       <c r="G28" t="b">
@@ -1687,45 +1685,43 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110286826</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110286973</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Previous experience with some of the following tools would be considered an advantage: scientific or statistical computing (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;, R), SQL...</t>
+          <t>Стек языков: PHP5, PHP7, PHP8, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Perl, Go, JS, Kotlin, Java, C-Object, Swift. Стек серверный технологий...</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Demonstrate use of data visualization (Power BI, Excel), and analytic tools (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;, R, SQL, KNIME). Collaborate with multifunctional teams (Marketing...</t>
+          <t>Техническое управление проектами(продуктами) компании, решение возникающих проблем, согласование принимаемых архитектурных решений, разбор инцидентов, оптимизация инфраструктуры. Участие во встречах по...</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>108444291</t>
+          <t>109139039</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Младший Back-end разработчик</t>
+          <t>Тестировщик</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>80000</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>100000</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2024-11-06T09:12:58+0300</t>
+          <t>2024-11-07T13:02:06+0300</t>
         </is>
       </c>
       <c r="G29" t="b">
@@ -1733,43 +1729,45 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108444291</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109139039</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Языки программирования &lt;highlighttext&gt;Python&lt;/highlighttext&gt;/Golang, C#. Понимание принципа работы REST API, HTTP и клиент-серверной архитектуры. Знание основ работы с реляционными...</t>
+          <t>Умение фиксировать результат тестирования и ошибки в понятном для разработчиков виде. Проведение review тестов. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; - как преимущество.</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Разработка микросервисов, которые обеспечивают работу разных частей большого проекта, например, обработку платежей или отправку уведомлений. Разработка REST API для обеспечения...</t>
+          <t xml:space="preserve">Написание тестов к разрабатываемым системам и сервисам. Формирование правил тестирования и сценариев тестирования. Участие в приемке и передаче нового функционала. </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>109139039</t>
+          <t>108444291</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Тестировщик</t>
+          <t>Младший Back-end разработчик</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0</v>
+        <v>100000</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2024-11-07T13:02:06+0300</t>
+          <t>2024-11-06T09:12:58+0300</t>
         </is>
       </c>
       <c r="G30" t="b">
@@ -1777,43 +1775,45 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109139039</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108444291</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Умение фиксировать результат тестирования и ошибки в понятном для разработчиков виде. Проведение review тестов. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; - как преимущество.</t>
+          <t>Языки программирования &lt;highlighttext&gt;Python&lt;/highlighttext&gt;/Golang, C#. Понимание принципа работы REST API, HTTP и клиент-серверной архитектуры. Знание основ работы с реляционными...</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Написание тестов к разрабатываемым системам и сервисам. Формирование правил тестирования и сценариев тестирования. Участие в приемке и передаче нового функционала. </t>
+          <t>Разработка микросервисов, которые обеспечивают работу разных частей большого проекта, например, обработку платежей или отправку уведомлений. Разработка REST API для обеспечения...</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>110332213</t>
+          <t>110219578</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Стажер / Аналитик данных</t>
+          <t>Junior IT специалист | Младший аналитик | Системный аналитик</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
+        <v>140000</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2024-11-07T16:32:18+0300</t>
+          <t>2024-11-06T11:32:46+0300</t>
         </is>
       </c>
       <c r="G31" t="b">
@@ -1821,43 +1821,45 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110332213</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110219578</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Имеете опыт работы с базами данных. Знаете и работаете с SQL и &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (желательно). Имеете опыт взаимодействия с системами класса...</t>
+          <t xml:space="preserve">Высшее образование (желательно техническое или математическое). Плюсом будет знание языков программирования (например, SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;). Понимание принципов работы реляционных баз данных. </t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Отдел информационных систем:</t>
+          <t>Сбор и анализ требований к системам. Разработка технических заданий. Участие в проектировании систем. Тестирование программного обеспечения.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>110352216</t>
+          <t>110286826</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Python-разработчик</t>
+          <t>Intern Data Analyst / Стажер - аналитик данных</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
-      <c r="E32" t="n">
-        <v>0</v>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2024-11-08T06:30:33+0300</t>
+          <t>2024-11-07T09:20:15+0300</t>
         </is>
       </c>
       <c r="G32" t="b">
@@ -1865,17 +1867,17 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110352216</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110286826</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Postgresql/Mysql;CSS - Bootstrap, Foundation, Materialize, препроцессоры SASS/SCSS/LESS. Асинхронное программирование на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; 3 (Asyncio, Twisted, etc..). </t>
+          <t>Previous experience with some of the following tools would be considered an advantage: scientific or statistical computing (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;, R), SQL...</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Разработка и поддержка собственных web-сервисов компании, внутренние технологические решения. Анализ требований и выявление потребностей конечных пользователей. Проработка архитектуры проектов...</t>
+          <t>Demonstrate use of data visualization (Power BI, Excel), and analytic tools (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;, R, SQL, KNIME). Collaborate with multifunctional teams (Marketing...</t>
         </is>
       </c>
     </row>
@@ -1974,28 +1976,26 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>110259069</t>
+          <t>110332213</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QA Engineer (Backend)</t>
+          <t>Стажер / Аналитик данных</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>150000</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2024-11-06T16:40:25+0300</t>
+          <t>2024-11-07T16:32:18+0300</t>
         </is>
       </c>
       <c r="G35" t="b">
@@ -2003,17 +2003,17 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110259069</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110332213</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Имеешь коммерческий опыт тестирования от 2 лет. Имеешь опыт работы на проекте с микросервисной архитектурой. Имеешь навыки работы с Postman...</t>
+          <t>Имеете опыт работы с базами данных. Знаете и работаете с SQL и &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (желательно). Имеете опыт взаимодействия с системами класса...</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Одна из ключевых команд — команда Search — занимается поисковой выдачей: определяет логику показа номерного фонда отелей и определяет правила скидок. </t>
+          <t>Отдел информационных систем:</t>
         </is>
       </c>
     </row>
@@ -2066,16 +2066,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>110235481</t>
+          <t>110259069</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Python-API разработчик</t>
+          <t>QA Engineer (Backend)</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>150000</v>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2024-11-06T12:46:39+0300</t>
+          <t>2024-11-06T16:40:25+0300</t>
         </is>
       </c>
       <c r="G37" t="b">
@@ -2095,45 +2095,43 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110235481</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110259069</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Учитывая специфику и особенности, мы сможем обеспечить для Вас. Специалиста со знанием &lt;highlighttext&gt;Python&lt;/highlighttext&gt; c опытом написания интеграционных сервисов. </t>
+          <t>Имеешь коммерческий опыт тестирования от 2 лет. Имеешь опыт работы на проекте с микросервисной архитектурой. Имеешь навыки работы с Postman...</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Компания "Делис Инфо" (включена в реестр отечественных ИТ-компаний) создает и развивает на российском рынке линейку продуктов собственной разработки по...</t>
+          <t xml:space="preserve">Одна из ключевых команд — команда Search — занимается поисковой выдачей: определяет логику показа номерного фонда отелей и определяет правила скидок. </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>110219578</t>
+          <t>110352216</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Junior IT специалист | Младший аналитик | Системный аналитик</t>
+          <t>Python-разработчик</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>80000</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>140000</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2024-11-06T11:32:46+0300</t>
+          <t>2024-11-08T06:30:33+0300</t>
         </is>
       </c>
       <c r="G38" t="b">
@@ -2141,36 +2139,36 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110219578</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110352216</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Высшее образование (желательно техническое или математическое). Плюсом будет знание языков программирования (например, SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;). Понимание принципов работы реляционных баз данных. </t>
+          <t xml:space="preserve">Postgresql/Mysql;CSS - Bootstrap, Foundation, Materialize, препроцессоры SASS/SCSS/LESS. Асинхронное программирование на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; 3 (Asyncio, Twisted, etc..). </t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Сбор и анализ требований к системам. Разработка технических заданий. Участие в проектировании систем. Тестирование программного обеспечения.</t>
+          <t>Разработка и поддержка собственных web-сервисов компании, внутренние технологические решения. Анализ требований и выявление потребностей конечных пользователей. Проработка архитектуры проектов...</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>108457731</t>
+          <t>110235481</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>DevOps-инженер</t>
+          <t>Python-API разработчик</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="D39" t="n">
-        <v>400000</v>
+        <v>150000</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2179,7 +2177,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2024-10-10T11:52:26+0300</t>
+          <t>2024-11-06T12:46:39+0300</t>
         </is>
       </c>
       <c r="G39" t="b">
@@ -2187,17 +2185,17 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108457731</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110235481</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Умение применять инструменты для работы с IaC (Ansible, Terraform). Понимание практик безопасной разработки (SSDL). Опыт разработки на языках &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Go...</t>
+          <t xml:space="preserve">Учитывая специфику и особенности, мы сможем обеспечить для Вас. Специалиста со знанием &lt;highlighttext&gt;Python&lt;/highlighttext&gt; c опытом написания интеграционных сервисов. </t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Участие в развитии практик DevOps в команде. Обеспечение CI/CD процессов (разработка pipeline, разворачивание сред). Администрирование инфраструктуры (PostgreSQL, Redis, Keyсloak...</t>
+          <t>Компания "Делис Инфо" (включена в реестр отечественных ИТ-компаний) создает и развивает на российском рынке линейку продуктов собственной разработки по...</t>
         </is>
       </c>
     </row>
@@ -2250,26 +2248,28 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>108811289</t>
+          <t>108457731</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Senior Backend Developer (Python)</t>
+          <t>DevOps-инженер</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
+        <v>400000</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2024-10-17T16:39:16+0300</t>
+          <t>2024-10-10T11:52:26+0300</t>
         </is>
       </c>
       <c r="G41" t="b">
@@ -2277,45 +2277,43 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108811289</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108457731</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт построения высоконагруженных сервисов и обеспечения их доступности и надёжности. Опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; от 3-х лет. </t>
+          <t>Умение применять инструменты для работы с IaC (Ansible, Terraform). Понимание практик безопасной разработки (SSDL). Опыт разработки на языках &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Go...</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Разрабатывать новые сервисы и активно участвовать в переходе на cloud native архитектуру. Проектировать архитектуру новых сервисов и оптимизировать производительность текущих. </t>
+          <t>Участие в развитии практик DevOps в команде. Обеспечение CI/CD процессов (разработка pipeline, разворачивание сред). Администрирование инфраструктуры (PostgreSQL, Redis, Keyсloak...</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>110262826</t>
+          <t>108811289</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Junior+ Python/Go разработчик</t>
+          <t>Senior Backend Developer (Python)</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>110000</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2024-11-06T17:46:48+0300</t>
+          <t>2024-10-17T16:39:16+0300</t>
         </is>
       </c>
       <c r="G42" t="b">
@@ -2323,43 +2321,45 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110262826</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108811289</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Опыт коммерческой разработки от 1 года. Владение &lt;highlighttext&gt;Python&lt;/highlighttext&gt; 2/3. Владение (My)SQL, конкретно. Написать запросы, достаточные для CRUD (SELECT...</t>
+          <t xml:space="preserve">Опыт построения высоконагруженных сервисов и обеспечения их доступности и надёжности. Опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; от 3-х лет. </t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Написание и поддержка интеграций (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;2, MySQL, SOAP/REST). Поддержка и развитие существующих клиент-серверных продуктов (&lt;highlighttext&gt;Python&lt;/highlighttext&gt; 3 + FastApi...</t>
+          <t xml:space="preserve">Разрабатывать новые сервисы и активно участвовать в переходе на cloud native архитектуру. Проектировать архитектуру новых сервисов и оптимизировать производительность текущих. </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>109221893</t>
+          <t>110262826</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Middle QA manual engineer (онлайн-кинотеатр Premier, Матч ТВ, сайты телеканалов)</t>
+          <t>Junior+ Python/Go разработчик</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
+        <v>110000</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2024-10-24T13:24:30+0300</t>
+          <t>2024-11-06T17:46:48+0300</t>
         </is>
       </c>
       <c r="G43" t="b">
@@ -2367,29 +2367,29 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109221893</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110262826</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Опыт работы с инструментами подмены/изменения запросов (снифферы) - Fiddler, Charles Proxy. Опыт ручного тестирования бэкенд части приложений (REST API, Postman...</t>
+          <t>Опыт коммерческой разработки от 1 года. Владение &lt;highlighttext&gt;Python&lt;/highlighttext&gt; 2/3. Владение (My)SQL, конкретно. Написать запросы, достаточные для CRUD (SELECT...</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Проведение тестирования нового функционала, интеграционного и регрессионного тестирования. Участие во встречах по оценке сложности задач. Написание тест-кейсов и чеклистов. </t>
+          <t>Написание и поддержка интеграций (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;2, MySQL, SOAP/REST). Поддержка и развитие существующих клиент-серверных продуктов (&lt;highlighttext&gt;Python&lt;/highlighttext&gt; 3 + FastApi...</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>110262015</t>
+          <t>110117743</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Web Backend Developer (Python)</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -2403,7 +2403,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2024-11-06T17:26:57+0300</t>
+          <t>2024-11-05T12:21:15+0300</t>
         </is>
       </c>
       <c r="G44" t="b">
@@ -2411,29 +2411,29 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110262015</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110117743</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Уверенное владение &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (от 3 лет). Опыт работы с Flask, понимание его экосистемы и лучших практик разработки. Знание и опыт...</t>
+          <t>&lt;highlighttext&gt;Python&lt;/highlighttext&gt; - flask/aiohttp/django, requests, SQLAlchemy, asyncio. Базовые навыки работы в cli, bash/zsh - SQL - написание сложных запросов (оконные функции...</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Разработка и поддержка веб-приложений на Flask. Интеграция с внешними API и внутренними сервисами. Оптимизация производительности приложений. Работа с базами...</t>
+          <t>Разработка скриптов для обработки кредитных заявок (Java, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, SQL). Интеграция новых источников данных (БКИ, телеком, различные реестры). Оптимизация и рефакторинг...</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>110416959</t>
+          <t>110262015</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Backend Developer (Python/FAST API)</t>
+          <t>Web Backend Developer (Python)</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2024-11-08T12:57:57+0300</t>
+          <t>2024-11-06T17:26:57+0300</t>
         </is>
       </c>
       <c r="G45" t="b">
@@ -2455,29 +2455,29 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110416959</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110262015</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Уверенное владение &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (FAST API и Flask). Опыт работы с highload сервисами. Понимание DjangoORM и миграций. Опыт разработки API, работы...</t>
+          <t>Уверенное владение &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (от 3 лет). Опыт работы с Flask, понимание его экосистемы и лучших практик разработки. Знание и опыт...</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Помогать выстраивать процессы в команде (стандарты и ревью кода, тесты, демо, ретро и т.д.). Разрабатывать новые продуктовые фичи, поступающие...</t>
+          <t>Разработка и поддержка веб-приложений на Flask. Интеграция с внешними API и внутренними сервисами. Оптимизация производительности приложений. Работа с базами...</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>110117743</t>
+          <t>110337472</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Python Developer</t>
+          <t>Младший аналитик</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2024-11-05T12:21:15+0300</t>
+          <t>2024-11-07T18:48:57+0300</t>
         </is>
       </c>
       <c r="G46" t="b">
@@ -2499,29 +2499,29 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110117743</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110337472</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>&lt;highlighttext&gt;Python&lt;/highlighttext&gt; - flask/aiohttp/django, requests, SQLAlchemy, asyncio. Базовые навыки работы в cli, bash/zsh - SQL - написание сложных запросов (оконные функции...</t>
+          <t>Высшее образование или проходишь последние курсы обучения (предпочтительно: математика, статистика, информатика). Готовность работать полный день в офисе 5/2 (для...</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Разработка скриптов для обработки кредитных заявок (Java, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, SQL). Интеграция новых источников данных (БКИ, телеком, различные реестры). Оптимизация и рефакторинг...</t>
+          <t>Разработка веб-форм для онлайн-опросов в нашем ПО с использованием скриптов. Работа с базами данных, полученных в ходе опросов...</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>109214915</t>
+          <t>110445717</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Стажер в отдел тестирования</t>
+          <t>Инженер интеграции данных</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2024-10-24T11:56:50+0300</t>
+          <t>2024-11-08T17:48:31+0300</t>
         </is>
       </c>
       <c r="G47" t="b">
@@ -2543,29 +2543,29 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109214915</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110445717</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Желателен опыт работы с Jira\Confluence. Желателен опыт в написании скриптов (Shell, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;). Желателен опыт работы с системами контроля версий...</t>
+          <t xml:space="preserve">Развитые аналитические навыки и умение эффективно решать сложные задачи. Будет плюсом: Опыт работы с &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и средствами автоматизации (например, AirFlow). </t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Выполнение ручного функционального тестирования новых версий продукта. Тестирование графических и консольных интерфейсов. Регистрация выявленных ошибок, описание и определение условий возникновения...</t>
+          <t xml:space="preserve">Реализацией и настройкой интеграций с внешними системами. Анализом и устранением ошибок в работе интеграций, включая анализ ошибок в хранимых процедурах. </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>110337472</t>
+          <t>110310787</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Младший аналитик</t>
+          <t>Стажер IT</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2024-11-07T18:48:57+0300</t>
+          <t>2024-11-07T12:23:55+0300</t>
         </is>
       </c>
       <c r="G48" t="b">
@@ -2587,45 +2587,43 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110337472</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110310787</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Высшее образование или проходишь последние курсы обучения (предпочтительно: математика, статистика, информатика). Готовность работать полный день в офисе 5/2 (для...</t>
+          <t>Аналитический склад ума, ответственность, исполнительность. Знания языков программирования: VBA, SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, C++, C#.</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Разработка веб-форм для онлайн-опросов в нашем ПО с использованием скриптов. Работа с базами данных, полученных в ходе опросов...</t>
+          <t>Участие в поддержке, настройке и разработке системы TDM Navigator.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>110037650</t>
+          <t>109221893</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Junior Тестировщик/QA Engineer</t>
+          <t>Middle QA manual engineer (онлайн-кинотеатр Premier, Матч ТВ, сайты телеканалов)</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E49" t="n">
+        <v>0</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2024-11-04T10:40:24+0300</t>
+          <t>2024-10-24T13:24:30+0300</t>
         </is>
       </c>
       <c r="G49" t="b">
@@ -2633,36 +2631,36 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110037650</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109221893</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Понимание структуры web-приложений. Знание английского языка B1. Умение работать с командой. Умение составлять ТЗ. Postman. DevTools. Figma. </t>
+          <t>Опыт работы с инструментами подмены/изменения запросов (снифферы) - Fiddler, Charles Proxy. Опыт ручного тестирования бэкенд части приложений (REST API, Postman...</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Тестирование сайтов, мобильных приложений и API в соответствии с ТЗ. Анализировать ТЗ к разрабатываемому продукту. Написание Bug-репортов.</t>
+          <t xml:space="preserve">Проведение тестирования нового функционала, интеграционного и регрессионного тестирования. Участие во встречах по оценке сложности задач. Написание тест-кейсов и чеклистов. </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>110038797</t>
+          <t>110037650</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Python-разработчик (Junior)</t>
+          <t>Junior Тестировщик/QA Engineer</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>150000</v>
+        <v>60000</v>
       </c>
       <c r="D50" t="n">
-        <v>180000</v>
+        <v>0</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2671,7 +2669,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2024-11-07T11:36:47+0300</t>
+          <t>2024-11-04T10:40:24+0300</t>
         </is>
       </c>
       <c r="G50" t="b">
@@ -2679,43 +2677,45 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110038797</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110037650</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание основ работы с FastAPI. Знание основ работы с PostgreSQL (MongoDB будет плюсом). Понимание принципов REST. </t>
+          <t xml:space="preserve">Понимание структуры web-приложений. Знание английского языка B1. Умение работать с командой. Умение составлять ТЗ. Postman. DevTools. Figma. </t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Участие в разработке и поддержке веб-приложений на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Помощь в интеграции сторонних сервисов и API. Поддержка существующего кода и...</t>
+          <t>Тестирование сайтов, мобильных приложений и API в соответствии с ТЗ. Анализировать ТЗ к разрабатываемому продукту. Написание Bug-репортов.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>110310787</t>
+          <t>110038797</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Стажер IT</t>
+          <t>Python-разработчик (Junior)</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
+        <v>180000</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2024-11-07T12:23:55+0300</t>
+          <t>2024-11-07T11:36:47+0300</t>
         </is>
       </c>
       <c r="G51" t="b">
@@ -2723,45 +2723,43 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110310787</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110038797</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Аналитический склад ума, ответственность, исполнительность. Знания языков программирования: VBA, SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, C++, C#.</t>
+          <t xml:space="preserve">Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание основ работы с FastAPI. Знание основ работы с PostgreSQL (MongoDB будет плюсом). Понимание принципов REST. </t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Участие в поддержке, настройке и разработке системы TDM Navigator.</t>
+          <t>Участие в разработке и поддержке веб-приложений на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Помощь в интеграции сторонних сервисов и API. Поддержка существующего кода и...</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>109974390</t>
+          <t>109214915</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Начинающий DevOps-инженер / Стажёр</t>
+          <t>Стажер в отдел тестирования</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>120000</v>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2024-11-02T19:43:47+0300</t>
+          <t>2024-10-24T11:56:50+0300</t>
         </is>
       </c>
       <c r="G52" t="b">
@@ -2769,17 +2767,17 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109974390</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109214915</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Тестовый отбор — выполнение кандидатами задач на знание базовых linux команд. Успешно прошедшие тестовые задания кандидаты переходят ко второму этапу.</t>
+          <t>Желателен опыт работы с Jira\Confluence. Желателен опыт в написании скриптов (Shell, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;). Желателен опыт работы с системами контроля версий...</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Зачисление в штат. Вашими должностными обязанностями будет: Перенос приложений в систему оркестрации Kubernetes; Автоматизация процессов разработки, тестирования и сборки релизного...</t>
+          <t>Выполнение ручного функционального тестирования новых версий продукта. Тестирование графических и консольных интерфейсов. Регистрация выявленных ошибок, описание и определение условий возникновения...</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2828,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>110261481</t>
+          <t>110416959</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>QA Engineer</t>
+          <t>Backend Developer (Python/FAST API)</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -2849,7 +2847,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2024-11-06T17:18:48+0300</t>
+          <t>2024-11-08T12:57:57+0300</t>
         </is>
       </c>
       <c r="G54" t="b">
@@ -2857,43 +2855,45 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110261481</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110416959</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>4. Базовое понимание принципов ООП. 5. Плюсом будет опыт работы с автотестами. Желательно: * знание стэка: &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, FastAPI, PostgreSQL, VueJS, JS.</t>
+          <t>Уверенное владение &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (FAST API и Flask). Опыт работы с highload сервисами. Понимание DjangoORM и миграций. Опыт разработки API, работы...</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Разрабатываем собственную платформу для управления видео и аудио информацией в магазинах, на транспорте, кафе и ресторанах. Занимаемся как доставкой и...</t>
+          <t>Помогать выстраивать процессы в команде (стандарты и ревью кода, тесты, демо, ретро и т.д.). Разрабатывать новые продуктовые фичи, поступающие...</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>110325608</t>
+          <t>109974390</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Python Developer</t>
+          <t>Начинающий DevOps-инженер / Стажёр</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
+        <v>120000</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2024-11-07T14:57:11+0300</t>
+          <t>2024-11-02T19:43:47+0300</t>
         </is>
       </c>
       <c r="G55" t="b">
@@ -2901,29 +2901,29 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110325608</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109974390</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Опыт работы на позиции разработчика от 2х лет. Отличное знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Отличное знание SQL. Отличное знание алгоритмов и структур...</t>
+          <t>Тестовый отбор — выполнение кандидатами задач на знание базовых linux команд. Успешно прошедшие тестовые задания кандидаты переходят ко второму этапу.</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Участвовать в разработке продукта: декомпозиция, оценка задач и их реализация. Взаимодействовать с членами команды, интеграторами платформ, заказчиками. Участвовать в разработке...</t>
+          <t>Зачисление в штат. Вашими должностными обязанностями будет: Перенос приложений в систему оркестрации Kubernetes; Автоматизация процессов разработки, тестирования и сборки релизного...</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>110319598</t>
+          <t>110261481</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Программист на Python</t>
+          <t>QA Engineer</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -2937,7 +2937,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2024-11-07T13:38:48+0300</t>
+          <t>2024-11-06T17:18:48+0300</t>
         </is>
       </c>
       <c r="G56" t="b">
@@ -2945,29 +2945,29 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110319598</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110261481</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Знание основ SQL. Опыт работы с реляционной БД (желательно PostgreSQL). Понимание как работает асихронность в &lt;highlighttext&gt;python&lt;/highlighttext&gt;. Желание развивать профессиональные навыки.</t>
+          <t>4. Базовое понимание принципов ООП. 5. Плюсом будет опыт работы с автотестами. Желательно: * знание стэка: &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, FastAPI, PostgreSQL, VueJS, JS.</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Написание backend части корпоративных сервисов на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Разработка новых и поддержка существующих сервисов. Участие в принятии архитектурных решений по проектам. </t>
+          <t>Разрабатываем собственную платформу для управления видео и аудио информацией в магазинах, на транспорте, кафе и ресторанах. Занимаемся как доставкой и...</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>110335772</t>
+          <t>110325608</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Младший аналитик данных / Junior data analyst</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2024-11-07T17:42:32+0300</t>
+          <t>2024-11-07T14:57:11+0300</t>
         </is>
       </c>
       <c r="G57" t="b">
@@ -2989,29 +2989,29 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110335772</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110325608</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Хороший SQL (PostgreSQL или MySQL, будет плюсом Clickhouse или другой диалект для работы с колоночной базой данных). - &lt;highlighttext&gt;Python&lt;/highlighttext&gt; для анализа...</t>
+          <t>Опыт работы на позиции разработчика от 2х лет. Отличное знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Отличное знание SQL. Отличное знание алгоритмов и структур...</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Решением задач бизнеса с помощью аналитики и BI. - Разработкой и реализацией моделей и алгоритмов обработки данных. - Созданием и поддержкой дэшбордов...</t>
+          <t>Участвовать в разработке продукта: декомпозиция, оценка задач и их реализация. Взаимодействовать с членами команды, интеграторами платформ, заказчиками. Участвовать в разработке...</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>110142668</t>
+          <t>110319598</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>QA Engineer</t>
+          <t>Программист на Python</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2024-11-05T16:50:17+0300</t>
+          <t>2024-11-07T13:38:48+0300</t>
         </is>
       </c>
       <c r="G58" t="b">
@@ -3033,45 +3033,43 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110142668</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110319598</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>Опыт в Web-тестировании. Опыт работы с API (Postman). Опыт работы с инструментами: DevTools, Postman. Знание Linux. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;.</t>
+          <t>Знание основ SQL. Опыт работы с реляционной БД (желательно PostgreSQL). Понимание как работает асихронность в &lt;highlighttext&gt;python&lt;/highlighttext&gt;. Желание развивать профессиональные навыки.</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Тестирование Web-приложений. Тестирование API (Postman). Создание тестовой документации (тест-кейсы, планы тестирования, чек-листы, матрицы покрытия требований). Анализ требований. </t>
+          <t xml:space="preserve">Написание backend части корпоративных сервисов на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Разработка новых и поддержка существующих сервисов. Участие в принятии архитектурных решений по проектам. </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>110288102</t>
+          <t>110335772</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Middle Python Developer</t>
+          <t>Младший аналитик данных / Junior data analyst</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>180000</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>260000</v>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2024-11-07T09:39:51+0300</t>
+          <t>2024-11-07T17:42:32+0300</t>
         </is>
       </c>
       <c r="G59" t="b">
@@ -3079,17 +3077,17 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110288102</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110335772</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Опыт асинхронного программирования в &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, опыт связывания асинхронного и синхронного кода. Опыт в применении аннотаций типов в &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание &lt;highlighttext&gt;python&lt;/highlighttext&gt;...</t>
+          <t>Хороший SQL (PostgreSQL или MySQL, будет плюсом Clickhouse или другой диалект для работы с колоночной базой данных). - &lt;highlighttext&gt;Python&lt;/highlighttext&gt; для анализа...</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Развитие существующих и разработка новых приложений в рамках продуктов компании. Оценка производительности. Поиск узких мест. Оптимизация кода. Написание технических спецификаций. </t>
+          <t>Решением задач бизнеса с помощью аналитики и BI. - Разработкой и реализацией моделей и алгоритмов обработки данных. - Созданием и поддержкой дэшбордов...</t>
         </is>
       </c>
     </row>
@@ -3140,26 +3138,28 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>110404251</t>
+          <t>110288102</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Инженер по тестированию (Middle)</t>
+          <t>Middle Python Developer</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0</v>
+        <v>260000</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2024-11-08T11:46:19+0300</t>
+          <t>2024-11-07T09:39:51+0300</t>
         </is>
       </c>
       <c r="G61" t="b">
@@ -3167,29 +3167,29 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110404251</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110288102</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>SQL на базовом уровне. Имеете опыт интеграционного тестирования web, знание инструментов. Имеете базовые знания программирования (&lt;highlighttext&gt;python&lt;/highlighttext&gt; в приоритете).</t>
+          <t>Опыт асинхронного программирования в &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, опыт связывания асинхронного и синхронного кода. Опыт в применении аннотаций типов в &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание &lt;highlighttext&gt;python&lt;/highlighttext&gt;...</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Тестирование продукта в рамках задач. Регрессионное тестирование. Взаимодействие с командами разработки, технической поддержки, автоматизации тестирования.</t>
+          <t xml:space="preserve">Развитие существующих и разработка новых приложений в рамках продуктов компании. Оценка производительности. Поиск узких мест. Оптимизация кода. Написание технических спецификаций. </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>110130854</t>
+          <t>110404251</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Стажер в Группу аналитики данных</t>
+          <t>Инженер по тестированию (Middle)</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2024-11-05T14:30:14+0300</t>
+          <t>2024-11-08T11:46:19+0300</t>
         </is>
       </c>
       <c r="G62" t="b">
@@ -3211,45 +3211,43 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110130854</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110404251</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Знание SQL (SELECT + JOIN + GROUPBY + Subqueries + UNION). Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; для анализа данных (pandas, numpy, plotly). </t>
+          <t>SQL на базовом уровне. Имеете опыт интеграционного тестирования web, знание инструментов. Имеете базовые знания программирования (&lt;highlighttext&gt;python&lt;/highlighttext&gt; в приоритете).</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Сбор и анализ требований заказчиков аналитики. Создание, корректировка и актуализация дашбордов в BI-системе компании. Осуществление ad-hoc аналитики. </t>
+          <t>Тестирование продукта в рамках задач. Регрессионное тестирование. Взаимодействие с командами разработки, технической поддержки, автоматизации тестирования.</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>108689213</t>
+          <t>110130854</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Prompt-engineer</t>
+          <t>Стажер в Группу аналитики данных</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>300000</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2024-11-08T16:11:15+0300</t>
+          <t>2024-11-05T14:30:14+0300</t>
         </is>
       </c>
       <c r="G63" t="b">
@@ -3257,45 +3255,43 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108689213</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110130854</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт в разработке. Будет плюсом: Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;/JavaScript. Опыт работы с моделями различной размерности 7b, 70b. </t>
+          <t xml:space="preserve">Знание SQL (SELECT + JOIN + GROUPBY + Subqueries + UNION). Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; для анализа данных (pandas, numpy, plotly). </t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Разработка и настройка чат-ботов на основе LLM в визуальном редакторе. Построение логики работы чат-ботов в соответствии с требованиями...</t>
+          <t xml:space="preserve">Сбор и анализ требований заказчиков аналитики. Создание, корректировка и актуализация дашбордов в BI-системе компании. Осуществление ad-hoc аналитики. </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>110264524</t>
+          <t>110142668</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Junior разработчик Kotlin / Java</t>
+          <t>QA Engineer</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>500</v>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2024-11-06T18:32:23+0300</t>
+          <t>2024-11-05T16:50:17+0300</t>
         </is>
       </c>
       <c r="G64" t="b">
@@ -3303,29 +3299,29 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110264524</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110142668</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>...технологии (по убыванию приоритетности: PHP, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, C#). Уверенное владение PHP (можно без объектного подхода), &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание HTML/CSS/Java Script...</t>
+          <t>Опыт в Web-тестировании. Опыт работы с API (Postman). Опыт работы с инструментами: DevTools, Postman. Знание Linux. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;.</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Разработка back-end для мобильных приложений, возможен минимальный front (без особой критики по дизайну и пр.). Android Studio/Kotlin, знание...</t>
+          <t xml:space="preserve">Тестирование Web-приложений. Тестирование API (Postman). Создание тестовой документации (тест-кейсы, планы тестирования, чек-листы, матрицы покрытия требований). Анализ требований. </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>110430976</t>
+          <t>110441537</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Data analyst / аналитик данных (Junior)</t>
+          <t>Data Analyst (Стажер)</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -3339,7 +3335,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2024-11-08T15:55:18+0300</t>
+          <t>2024-11-08T16:44:33+0300</t>
         </is>
       </c>
       <c r="G65" t="b">
@@ -3347,36 +3343,36 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110430976</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110441537</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Аналитические способности, умение находить нужные данные и задавать правильные вопросы к данным. &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Навыки визуализации данных. Релевантный опыт. </t>
+          <t>Огромное желание обучаться и расти в IT компании. Так же важны базовое знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и SQL.</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Регулярная подготовка аналитических отчетов по результатам маркетинговых кампаний и по продуктовой аналитике. Участие в создании инфраструктуры для сбора, хранения и...</t>
+          <t>BI системы (такие как Apache Superset, Yandex Datalens, Metabase и прч.) - создание и наполнение дашбордов. Написание SQL запросов, поддержка баз...</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>110382689</t>
+          <t>108689213</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Python-developer</t>
+          <t>Prompt-engineer</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>175000</v>
+        <v>100000</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3385,7 +3381,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2024-11-08T10:04:03+0300</t>
+          <t>2024-11-08T16:11:15+0300</t>
         </is>
       </c>
       <c r="G66" t="b">
@@ -3393,43 +3389,45 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110382689</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108689213</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>Делать лучший продукт в России. Уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, ООП. Опыт работы с PostgreSQL: построение оптимальных sql-запросов (без использования ORM...</t>
+          <t xml:space="preserve">Опыт в разработке. Будет плюсом: Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;/JavaScript. Опыт работы с моделями различной размерности 7b, 70b. </t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Разработка высоконагруженного финансового приложения. - Реализация сервиса доставки. - Развитие и сопровождение высоконагруженного приложения фиксации активности пользователей.</t>
+          <t>Разработка и настройка чат-ботов на основе LLM в визуальном редакторе. Построение логики работы чат-ботов в соответствии с требованиями...</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>110337950</t>
+          <t>110264524</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Лингвист</t>
+          <t>Junior разработчик Kotlin / Java</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
-      </c>
-      <c r="E67" t="n">
-        <v>0</v>
+        <v>500</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2024-11-07T19:27:03+0300</t>
+          <t>2024-11-06T18:32:23+0300</t>
         </is>
       </c>
       <c r="G67" t="b">
@@ -3437,45 +3435,43 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110337950</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110264524</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>Дополнительными плюсами будут: Владение языком регулярных выражений (regexp). Опыт работы с ОС Linux, с языками Bash, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Lua.</t>
+          <t>...технологии (по убыванию приоритетности: PHP, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, C#). Уверенное владение PHP (можно без объектного подхода), &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание HTML/CSS/Java Script...</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кастомизация технологий контентного анализа под требования заказчика. Работа с заказчиками, телефонные переговоры, встречи в режиме ВКС, выезды, командировки (редко). </t>
+          <t>Разработка back-end для мобильных приложений, возможен минимальный front (без особой критики по дизайну и пр.). Android Studio/Kotlin, знание...</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>110420382</t>
+          <t>110337950</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Разработчик ботов/удаленка/в штат</t>
+          <t>Лингвист</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E68" t="n">
+        <v>0</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2024-11-08T13:46:26+0300</t>
+          <t>2024-11-07T19:27:03+0300</t>
         </is>
       </c>
       <c r="G68" t="b">
@@ -3483,33 +3479,33 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110420382</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110337950</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>Желательно знание языка программирования &lt;highlighttext&gt;Python&lt;/highlighttext&gt; / JavaScript и основных библиотек для работы с чат-ботами, таких как &lt;highlighttext&gt;python&lt;/highlighttext&gt;-telegram-bot, Flask...</t>
+          <t>Дополнительными плюсами будут: Владение языком регулярных выражений (regexp). Опыт работы с ОС Linux, с языками Bash, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Lua.</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Разработка телеграмм-ботов, вотсап-ботов, разной направленности: Чат-боты. Юзер-боты. Настройка интеграций с системой AMO CRM Интеграция ИИ. Парсеры. </t>
+          <t xml:space="preserve">Кастомизация технологий контентного анализа под требования заказчика. Работа с заказчиками, телефонные переговоры, встречи в режиме ВКС, выезды, командировки (редко). </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>110372046</t>
+          <t>109077437</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Разработчик Python, Django</t>
+          <t>Финансовый аналитик</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>80000</v>
+        <v>400000</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
@@ -3521,7 +3517,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2024-11-08T09:08:24+0300</t>
+          <t>2024-11-07T18:57:47+0300</t>
         </is>
       </c>
       <c r="G69" t="b">
@@ -3529,43 +3525,45 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110372046</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109077437</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>Вы получаете востребованный опыт на современном стеке, развитие в кругу единомышленников. Ключевое требование - уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Django на проектах с...</t>
+          <t>Высшее образование в области экономики/математики. Продвинутый уровень владения MS Excel (обязательно). Навыки SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (желательно). Базовое понимание МСФО и...</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>На текущий момент реализовали дата-ядро системы на стеке PostgreSQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Datalens. Уперлись в большое количество ручных операций и приняли...</t>
+          <t xml:space="preserve">Построение и поддержка финансовых моделей компании. Подготовка бюджета компании на полугодовой основе и план-факт анализ на ежемесячной основе. </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>110425944</t>
+          <t>110372046</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Python developer / Python разработчик</t>
+          <t>Разработчик Python, Django</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="D70" t="n">
         <v>0</v>
       </c>
-      <c r="E70" t="n">
-        <v>0</v>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2024-11-08T15:10:17+0300</t>
+          <t>2024-11-08T09:08:24+0300</t>
         </is>
       </c>
       <c r="G70" t="b">
@@ -3573,33 +3571,33 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110425944</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110372046</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>Опытом разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;3. Глубокими знаниями и практическим опытом работы с Asyncio. Уверенными знаниями Linux. Умением работать в команде...</t>
+          <t>Вы получаете востребованный опыт на современном стеке, развитие в кругу единомышленников. Ключевое требование - уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Django на проектах с...</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Разработка и поддержка приложений на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;3 с использованием Asyncio. Оптимизация существующего кода и улучшение производительности приложений. Взаимодействие с командой...</t>
+          <t>На текущий момент реализовали дата-ядро системы на стеке PostgreSQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Datalens. Уперлись в большое количество ручных операций и приняли...</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>109077437</t>
+          <t>110382689</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Финансовый аналитик</t>
+          <t>Python-developer</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>400000</v>
+        <v>175000</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
@@ -3611,7 +3609,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2024-11-07T18:57:47+0300</t>
+          <t>2024-11-08T10:04:03+0300</t>
         </is>
       </c>
       <c r="G71" t="b">
@@ -3619,17 +3617,17 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109077437</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110382689</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>Высшее образование в области экономики/математики. Продвинутый уровень владения MS Excel (обязательно). Навыки SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (желательно). Базовое понимание МСФО и...</t>
+          <t>Делать лучший продукт в России. Уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, ООП. Опыт работы с PostgreSQL: построение оптимальных sql-запросов (без использования ORM...</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Построение и поддержка финансовых моделей компании. Подготовка бюджета компании на полугодовой основе и план-факт анализ на ежемесячной основе. </t>
+          <t>Разработка высоконагруженного финансового приложения. - Реализация сервиса доставки. - Развитие и сопровождение высоконагруженного приложения фиксации активности пользователей.</t>
         </is>
       </c>
     </row>
@@ -3680,12 +3678,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>110153452</t>
+          <t>108800548</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Python Developer в Краткосрочную аренду</t>
+          <t>Junior Python developer</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -3699,7 +3697,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2024-11-05T17:45:11+0300</t>
+          <t>2024-10-17T14:03:15+0300</t>
         </is>
       </c>
       <c r="G73" t="b">
@@ -3707,36 +3705,36 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110153452</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108800548</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Имеете опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; 3.X. Понимаете механику языка &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и сопутствующих инструментов (pytest, mypy, poetry, flake8). </t>
+          <t>Опыт работы с &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, SQL обязателен. Использование в своих проектах/пет-проектах асинхронные фреймворки (fastapi, aiohttp). Опыт работы с одной...</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Реализовывать высоконагруженные и производительные сервисы на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Участвовать в проектировании архитектуры, выработке решений по отказоустойчивости и производительности. Интегрироваться с партнерами...</t>
+          <t>Когда-то Циан был просто таблицей в Excel, в которой хранились квартиры, выставленные на продажу. Сейчас это самый большой маркетплейс...</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>108275731</t>
+          <t>109480482</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Тестировщик ПО</t>
+          <t>Backend-разработчик</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>90000</v>
+        <v>150000</v>
       </c>
       <c r="D74" t="n">
-        <v>140000</v>
+        <v>180000</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -3745,7 +3743,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2024-11-06T12:45:45+0300</t>
+          <t>2024-11-06T17:14:26+0300</t>
         </is>
       </c>
       <c r="G74" t="b">
@@ -3753,45 +3751,43 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108275731</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109480482</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Знание bash, &lt;highlighttext&gt;python&lt;/highlighttext&gt;, sql. Умение писать скрипты на Bash для автоматизации тестирования. Опыт написания тестов и автоматизации тестирования на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. </t>
+          <t xml:space="preserve">&lt;highlighttext&gt;Python&lt;/highlighttext&gt; 3.9-3.11 (в идеале от 1,5 лет опыта). Django 3.2-4.2. DRF. Celery. SQLAlchemy. </t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Тестирование и сопровождение системы документооборота (госсектор). - Разработка сценариев тестирования с применением &lt;highlighttext&gt;python&lt;/highlighttext&gt; и sql. - Тестирование микросервисов. - Поиск и устранение ошибок...</t>
+          <t>Написание кода по всем действующим backend продуктам. Поддержание существующего функционала (REST API для приложений, бизнес логика для бэк-офиса, панель...</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>110265443</t>
+          <t>110153452</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Data аналитик</t>
+          <t>Python Developer в Краткосрочную аренду</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>180000</v>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2024-11-06T19:31:57+0300</t>
+          <t>2024-11-08T17:45:11+0300</t>
         </is>
       </c>
       <c r="G75" t="b">
@@ -3799,43 +3795,45 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110265443</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110153452</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Анализировали данные на SQL и &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знаете статистику и базу для A/B-тестирования. Проверяете результаты и качество своей работы. </t>
+          <t xml:space="preserve">Имеете опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; 3.X. Понимаете механику языка &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и сопутствующих инструментов (pytest, mypy, poetry, flake8). </t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Искать точки роста и возможности для оптимизации процессов работы с данными для всех департаментов компании. Участвовать в построении DWH. </t>
+          <t>Реализовывать высоконагруженные и производительные сервисы на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Участвовать в проектировании архитектуры, выработке решений по отказоустойчивости и производительности. Интегрироваться с партнерами...</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>109189148</t>
+          <t>110265443</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Разработчик Python</t>
+          <t>Data аналитик</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
-      </c>
-      <c r="E76" t="n">
-        <v>0</v>
+        <v>180000</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2024-10-24T08:42:18+0300</t>
+          <t>2024-11-06T19:31:57+0300</t>
         </is>
       </c>
       <c r="G76" t="b">
@@ -3843,43 +3841,45 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109189148</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110265443</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>Навыки, которыми нужно владеть: Опыт разработки &lt;highlighttext&gt;Python&lt;/highlighttext&gt; от 3-х лет. Понимание OS Linux на уровне администратора. Умение работать в...</t>
+          <t xml:space="preserve">Анализировали данные на SQL и &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знаете статистику и базу для A/B-тестирования. Проверяете результаты и качество своей работы. </t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Участие в разработке современного решения на стыке сетевых технологий и продуктов в области кибербезопасности. Разработка модулей управления фаерволом под Linux. </t>
+          <t xml:space="preserve">Искать точки роста и возможности для оптимизации процессов работы с данными для всех департаментов компании. Участвовать в построении DWH. </t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>108800548</t>
+          <t>108275731</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Junior Python developer</t>
+          <t>Тестировщик ПО</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
-      </c>
-      <c r="E77" t="n">
-        <v>0</v>
+        <v>140000</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2024-10-17T14:03:15+0300</t>
+          <t>2024-11-06T12:45:45+0300</t>
         </is>
       </c>
       <c r="G77" t="b">
@@ -3887,45 +3887,43 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108800548</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108275731</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>Опыт работы с &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, SQL обязателен. Использование в своих проектах/пет-проектах асинхронные фреймворки (fastapi, aiohttp). Опыт работы с одной...</t>
+          <t xml:space="preserve">Знание bash, &lt;highlighttext&gt;python&lt;/highlighttext&gt;, sql. Умение писать скрипты на Bash для автоматизации тестирования. Опыт написания тестов и автоматизации тестирования на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. </t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Когда-то Циан был просто таблицей в Excel, в которой хранились квартиры, выставленные на продажу. Сейчас это самый большой маркетплейс...</t>
+          <t>Тестирование и сопровождение системы документооборота (госсектор). - Разработка сценариев тестирования с применением &lt;highlighttext&gt;python&lt;/highlighttext&gt; и sql. - Тестирование микросервисов. - Поиск и устранение ошибок...</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>108828750</t>
+          <t>109189148</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Backend разработчик</t>
+          <t>Разработчик Python</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
         <v>0</v>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E78" t="n">
+        <v>0</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2024-10-18T09:32:09+0300</t>
+          <t>2024-10-24T08:42:18+0300</t>
         </is>
       </c>
       <c r="G78" t="b">
@@ -3933,43 +3931,45 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108828750</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109189148</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Знание SQL. Опыт проектирования БД от 1 года. Опыт работы с какой либо СУБД (желательно PostgreSQL). Навыки алгоритмизации. </t>
+          <t>Навыки, которыми нужно владеть: Опыт разработки &lt;highlighttext&gt;Python&lt;/highlighttext&gt; от 3-х лет. Понимание OS Linux на уровне администратора. Умение работать в...</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Анализ задач и проектирование под них БД. Разработка бизнес логики под требования компании (имеется собственная платформа). Внедрение и поддержка новых...</t>
+          <t xml:space="preserve">Участие в разработке современного решения на стыке сетевых технологий и продуктов в области кибербезопасности. Разработка модулей управления фаерволом под Linux. </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>110287206</t>
+          <t>109364540</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Junior QA</t>
+          <t>Стажер Python-разработчик</t>
         </is>
       </c>
       <c r="C79" t="n">
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E79" t="n">
-        <v>0</v>
+        <v>80000</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2024-11-07T09:26:43+0300</t>
+          <t>2024-10-26T22:17:31+0300</t>
         </is>
       </c>
       <c r="G79" t="b">
@@ -3977,45 +3977,43 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110287206</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109364540</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>Внимательность к деталям. Знание жизненного цикла ПО. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; на базовом уровне. Знание SQL на уровне средний и выше.</t>
+          <t>Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и понимание основ ООП. Желателен опыт работы с библиотеками для работы с PDF и инструментами для распознавания...</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Составление тест-плана. Оформление тест-кейсов. Проведение тестирования. Оформление контрольных точек для шаблона поставки. Автоматизация тестирования.</t>
+          <t>Ищем начинающего &lt;highlighttext&gt;Python&lt;/highlighttext&gt;-разработчика для работы над проектом по оцифровке PDF-документов. Задача — доработка и создание обработчиков для различных типов...</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>110116779</t>
+          <t>110081936</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Программист-разработчик (начинающий Junior)</t>
+          <t>QA engineer (ручное тестирование)</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E80" t="n">
+        <v>0</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2024-11-05T12:10:24+0300</t>
+          <t>2024-11-05T06:07:31+0300</t>
         </is>
       </c>
       <c r="G80" t="b">
@@ -4023,36 +4021,36 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110116779</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110081936</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>Писать техническую документацию, зарабатывая баллы в карму от коллег, которые перестанут теряться в коде. Будет круто, если ты имеешь небольшой...</t>
+          <t xml:space="preserve">Умение анализировать логи для диагностики проблем. - Базовые навыки программирования или автоматизации тестов (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Shell-скрипты). - Опыт работы с Linux. </t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Используя магию, предсказываем будущее: на основе сквозной аналитики прогнозируем, когда нужная партия угля будет готова к погрузке на борт судна. - </t>
+          <t>Формирование планов тестирования и тест-кейсов. Проведение функционального, регрессионного и нагрузочного тестирования. Выполнение тестирования API. Проверка UI/UX на соответствие...</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>110190520</t>
+          <t>110116779</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>QA-инженер \ QA-engineer</t>
+          <t>Программист-разработчик (начинающий Junior)</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>100000</v>
+        <v>30000</v>
       </c>
       <c r="D81" t="n">
-        <v>130000</v>
+        <v>0</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -4061,7 +4059,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2024-11-06T04:07:41+0300</t>
+          <t>2024-11-05T12:10:24+0300</t>
         </is>
       </c>
       <c r="G81" t="b">
@@ -4069,45 +4067,43 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110190520</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110116779</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>Знания теории и принципов тестирования ПО. Опыт тестирования ПО (желательно от 2 лет). Написание и поддержка автотестов. Навыки работы с...</t>
+          <t>Писать техническую документацию, зарабатывая баллы в карму от коллег, которые перестанут теряться в коде. Будет круто, если ты имеешь небольшой...</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>...взаимодействие с командой разработки. Составление test cases. Написание и поддержка автотестов (java, kotlin, kotlin-js, &lt;highlighttext&gt;python&lt;/highlighttext&gt;, spectron и т. д.).</t>
+          <t xml:space="preserve">Используя магию, предсказываем будущее: на основе сквозной аналитики прогнозируем, когда нужная партия угля будет готова к погрузке на борт судна. - </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>110236998</t>
+          <t>110287206</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Junior DevOps (Python, Linux)</t>
+          <t>Junior QA</t>
         </is>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>85000</v>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2024-11-06T12:57:23+0300</t>
+          <t>2024-11-07T09:26:43+0300</t>
         </is>
       </c>
       <c r="G82" t="b">
@@ -4115,39 +4111,45 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110236998</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110287206</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание Linux. Приветствуется: Любой опыт работы с облаками и Kubernetes. Возможность оформления АйТи-отсрочки от армии (для военнообязанных).</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr"/>
+          <t>Внимательность к деталям. Знание жизненного цикла ПО. Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; на базовом уровне. Знание SQL на уровне средний и выше.</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Составление тест-плана. Оформление тест-кейсов. Проведение тестирования. Оформление контрольных точек для шаблона поставки. Автоматизация тестирования.</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>110081936</t>
+          <t>108828750</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>QA engineer (ручное тестирование)</t>
+          <t>Backend разработчик</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
       </c>
-      <c r="E83" t="n">
-        <v>0</v>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2024-11-05T06:07:31+0300</t>
+          <t>2024-10-18T09:32:09+0300</t>
         </is>
       </c>
       <c r="G83" t="b">
@@ -4155,36 +4157,36 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110081936</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=108828750</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Умение анализировать логи для диагностики проблем. - Базовые навыки программирования или автоматизации тестов (&lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Shell-скрипты). - Опыт работы с Linux. </t>
+          <t xml:space="preserve">Знание SQL. Опыт проектирования БД от 1 года. Опыт работы с какой либо СУБД (желательно PostgreSQL). Навыки алгоритмизации. </t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Формирование планов тестирования и тест-кейсов. Проведение функционального, регрессионного и нагрузочного тестирования. Выполнение тестирования API. Проверка UI/UX на соответствие...</t>
+          <t>Анализ задач и проектирование под них БД. Разработка бизнес логики под требования компании (имеется собственная платформа). Внедрение и поддержка новых...</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>109364540</t>
+          <t>110262767</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Стажер Python-разработчик</t>
+          <t>QA ручной тестировщик (проект)</t>
         </is>
       </c>
       <c r="C84" t="n">
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>80000</v>
+        <v>130000</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -4193,7 +4195,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2024-10-26T22:17:31+0300</t>
+          <t>2024-11-06T17:45:10+0300</t>
         </is>
       </c>
       <c r="G84" t="b">
@@ -4201,17 +4203,17 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109364540</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110262767</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и понимание основ ООП. Желателен опыт работы с библиотеками для работы с PDF и инструментами для распознавания...</t>
+          <t>Желание учиться и развиваться в области тестирования. Будет плюсом: - Понимание работы &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, JS Vue/Nuxt. - Знания и опыт использования автоматизированных...</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Ищем начинающего &lt;highlighttext&gt;Python&lt;/highlighttext&gt;-разработчика для работы над проектом по оцифровке PDF-документов. Задача — доработка и создание обработчиков для различных типов...</t>
+          <t xml:space="preserve">Ручное тестирование эндпоинтов API и верификация структур по swagger-спецификации. - Выполнение ручного тестирования веб-приложений и мобильных приложений. - </t>
         </is>
       </c>
     </row>
@@ -4262,19 +4264,19 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>110262767</t>
+          <t>110256732</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>QA ручной тестировщик (проект)</t>
+          <t>BI-аналитик</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="D86" t="n">
-        <v>130000</v>
+        <v>0</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -4283,7 +4285,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2024-11-06T17:45:10+0300</t>
+          <t>2024-11-06T16:05:17+0300</t>
         </is>
       </c>
       <c r="G86" t="b">
@@ -4291,33 +4293,33 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110262767</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110256732</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>Желание учиться и развиваться в области тестирования. Будет плюсом: - Понимание работы &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, JS Vue/Nuxt. - Знания и опыт использования автоматизированных...</t>
+          <t>знание математической статистики и теории вероятностей. - знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (pandas, NumPy, matplotlib, Sklearn) и других BI-систем будет плюсом. - высшее образование.</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ручное тестирование эндпоинтов API и верификация структур по swagger-спецификации. - Выполнение ручного тестирования веб-приложений и мобильных приложений. - </t>
+          <t>развитие и поддержка существующей отчетности, разработка отчетов «с нуля». - сбор требований от заказчиков отчетов. - сбор и интеграция данных из различных...</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>110256732</t>
+          <t>110420382</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>BI-аналитик</t>
+          <t>Разработчик ботов/удаленка/в штат</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>400000</v>
+        <v>40000</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
@@ -4329,7 +4331,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2024-11-06T16:05:17+0300</t>
+          <t>2024-11-08T13:46:26+0300</t>
         </is>
       </c>
       <c r="G87" t="b">
@@ -4337,17 +4339,17 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110256732</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110420382</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>знание математической статистики и теории вероятностей. - знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (pandas, NumPy, matplotlib, Sklearn) и других BI-систем будет плюсом. - высшее образование.</t>
+          <t>Желательно знание языка программирования &lt;highlighttext&gt;Python&lt;/highlighttext&gt; / JavaScript и основных библиотек для работы с чат-ботами, таких как &lt;highlighttext&gt;python&lt;/highlighttext&gt;-telegram-bot, Flask...</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>развитие и поддержка существующей отчетности, разработка отчетов «с нуля». - сбор требований от заказчиков отчетов. - сбор и интеграция данных из различных...</t>
+          <t xml:space="preserve">Разработка телеграмм-ботов, вотсап-ботов, разной направленности: Чат-боты. Юзер-боты. Настройка интеграций с системой AMO CRM Интеграция ИИ. Парсеры. </t>
         </is>
       </c>
     </row>
@@ -4444,28 +4446,28 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>110227768</t>
+          <t>109158236</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Middle Frontend-разработчик</t>
+          <t>Python (Django) Разработчик</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1200</v>
+        <v>100000</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>250000</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>RUR</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2024-11-06T12:12:34+0300</t>
+          <t>2024-10-23T17:43:43+0300</t>
         </is>
       </c>
       <c r="G90" t="b">
@@ -4473,43 +4475,45 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110227768</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109158236</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>...для управления состоянием. Опыт с инструментами сборки, такими как Webpack или Vite. Знание CI/CD инструментов. Знание C, C++, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;.</t>
+          <t xml:space="preserve">Понимать продукт, вникать в бизнес-процессы. Опыт &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (Django) Backend разработки от 2-х лет. Опыт работы с Django Templates. </t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Разработка новых пользовательских интерфейсов с использованием React или Vue.js. Поддержка существующих фронтенд-приложений. Написание тестов для обеспечения качества кода. </t>
+          <t>Разработка и поддержка сервиса аналитики маркетплейсов на Django. Предлагать архитектурные решения, участвовать в проектировании архитектуры продукта. Мониторить производительность, оптимизировать где...</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>110335683</t>
+          <t>110190520</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Ведущий тестировщик</t>
+          <t>QA-инженер \ QA-engineer</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0</v>
+        <v>130000</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2024-11-07T17:40:40+0300</t>
+          <t>2024-11-06T04:07:41+0300</t>
         </is>
       </c>
       <c r="G91" t="b">
@@ -4517,43 +4521,45 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110335683</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110190520</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>...Robot, Cucumber, SpecFlow, Fit[nesse] и т.д.). Уверенное знание одного из языков программирования (Java/&lt;highlighttext&gt;Python&lt;/highlighttext&gt;/Golang). Навыки автоматизации тестирования.</t>
+          <t>Знания теории и принципов тестирования ПО. Опыт тестирования ПО (желательно от 2 лет). Написание и поддержка автотестов. Навыки работы с...</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Сбор, анализ и тестирование требований, планирование и выдача оценок, подготовка тестовых сред и тестовых окружений. Исследовательское тестирование, консультация разработчиков и...</t>
+          <t>...взаимодействие с командой разработки. Составление test cases. Написание и поддержка автотестов (java, kotlin, kotlin-js, &lt;highlighttext&gt;python&lt;/highlighttext&gt;, spectron и т. д.).</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>110126573</t>
+          <t>110236998</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Аналитик / помощник аналитика (можно удаленно)</t>
+          <t>Junior DevOps (Python, Linux)</t>
         </is>
       </c>
       <c r="C92" t="n">
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
-      </c>
-      <c r="E92" t="n">
-        <v>0</v>
+        <v>85000</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2024-11-05T13:37:15+0300</t>
+          <t>2024-11-06T12:57:23+0300</t>
         </is>
       </c>
       <c r="G92" t="b">
@@ -4561,45 +4567,39 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110126573</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110236998</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t xml:space="preserve">В поиске аналитика / помощника аналитика. Желательно с опытом в области аналитики маркетинга, трафика, отделов продаж, моб.приложений или сайтов. </t>
-        </is>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>...Аналитика (GTM, GA, BigQuery, коллтрекинги, Excel); Аналитика отдела продаж; Программирование SQL, Js, html, php, R, &lt;highlighttext&gt;python&lt;/highlighttext&gt;; Интеграция CRM и сервисов.</t>
-        </is>
-      </c>
+          <t>Знание &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Знание Linux. Приветствуется: Любой опыт работы с облаками и Kubernetes. Возможность оформления АйТи-отсрочки от армии (для военнообязанных).</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>109158236</t>
+          <t>110335683</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Python (Django) Разработчик</t>
+          <t>Ведущий тестировщик</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>250000</v>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2024-10-23T17:43:43+0300</t>
+          <t>2024-11-07T17:40:40+0300</t>
         </is>
       </c>
       <c r="G93" t="b">
@@ -4607,45 +4607,43 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109158236</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110335683</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t xml:space="preserve">Понимать продукт, вникать в бизнес-процессы. Опыт &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (Django) Backend разработки от 2-х лет. Опыт работы с Django Templates. </t>
+          <t>...Robot, Cucumber, SpecFlow, Fit[nesse] и т.д.). Уверенное знание одного из языков программирования (Java/&lt;highlighttext&gt;Python&lt;/highlighttext&gt;/Golang). Навыки автоматизации тестирования.</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Разработка и поддержка сервиса аналитики маркетплейсов на Django. Предлагать архитектурные решения, участвовать в проектировании архитектуры продукта. Мониторить производительность, оптимизировать где...</t>
+          <t>Сбор, анализ и тестирование требований, планирование и выдача оценок, подготовка тестовых сред и тестовых окружений. Исследовательское тестирование, консультация разработчиков и...</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>110202463</t>
+          <t>110126573</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Тестировщик — стажер в Сбер</t>
+          <t>Аналитик / помощник аналитика (можно удаленно)</t>
         </is>
       </c>
       <c r="C94" t="n">
         <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>71800</v>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2024-11-06T09:51:26+0300</t>
+          <t>2024-11-05T13:37:15+0300</t>
         </is>
       </c>
       <c r="G94" t="b">
@@ -4653,43 +4651,45 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110202463</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110126573</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>Необходимые навыки: — Ansible. — Apache Kafka. — OpenShift. — REST API. — понимание микросервисной архитектуры.</t>
+          <t xml:space="preserve">В поиске аналитика / помощника аналитика. Желательно с опытом в области аналитики маркетинга, трафика, отделов продаж, моб.приложений или сайтов. </t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t xml:space="preserve">изучать характеристики нагрузочных тестов. — измерять параметры при запуске тестов и их влияние. — производить подготовку стенда перед запуском нагрузочного тестирования. — </t>
+          <t>...Аналитика (GTM, GA, BigQuery, коллтрекинги, Excel); Аналитика отдела продаж; Программирование SQL, Js, html, php, R, &lt;highlighttext&gt;python&lt;/highlighttext&gt;; Интеграция CRM и сервисов.</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>110291970</t>
+          <t>110227768</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Аналитик баз данных (junior)</t>
+          <t>Middle Frontend-разработчик</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
       </c>
-      <c r="E95" t="n">
-        <v>0</v>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2024-11-07T10:27:11+0300</t>
+          <t>2024-11-06T12:12:34+0300</t>
         </is>
       </c>
       <c r="G95" t="b">
@@ -4697,17 +4697,17 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110291970</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110227768</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>Высшее образование (Математическое/Информационные технологии). Понимание архитектуры данных. Опыт работы: с SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (про часть работы с бд), Airflow, Superset...</t>
+          <t>...для управления состоянием. Опыт с инструментами сборки, такими как Webpack или Vite. Знание CI/CD инструментов. Знание C, C++, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;.</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Анализ данных из систем-источников ( Postgres, greenplum). Построение отчетности на основе бизнес требований ( &lt;highlighttext&gt;Python&lt;/highlighttext&gt; , Airflow, superset ). Подготовка технической документации и...</t>
+          <t xml:space="preserve">Разработка новых пользовательских интерфейсов с использованием React или Vue.js. Поддержка существующих фронтенд-приложений. Написание тестов для обеспечения качества кода. </t>
         </is>
       </c>
     </row>
@@ -4760,28 +4760,26 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>109420687</t>
+          <t>110430976</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Python-разработчик (Junior)</t>
+          <t>Data analyst / аналитик данных (Junior)</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>75000</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
       </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E97" t="n">
+        <v>0</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2024-11-08T11:17:36+0300</t>
+          <t>2024-11-08T15:55:18+0300</t>
         </is>
       </c>
       <c r="G97" t="b">
@@ -4789,45 +4787,43 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109420687</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110430976</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t xml:space="preserve">Уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Опыт работы с FastAPI / Flask. Знание основ SQL. Опыт работы с Linux. Понимание основ работы с сетями. </t>
+          <t xml:space="preserve">Аналитические способности, умение находить нужные данные и задавать правильные вопросы к данным. &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Навыки визуализации данных. Релевантный опыт. </t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Разработкой API. Разработкой и реализацией Unit-тестов. Написанием технической документации.</t>
+          <t>Регулярная подготовка аналитических отчетов по результатам маркетинговых кампаний и по продуктовой аналитике. Участие в создании инфраструктуры для сбора, хранения и...</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>109564037</t>
+          <t>110291970</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Junior Backend-разработчик Django</t>
+          <t>Аналитик баз данных (junior)</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="D98" t="n">
         <v>0</v>
       </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+      <c r="E98" t="n">
+        <v>0</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2024-11-07T15:56:31+0300</t>
+          <t>2024-11-07T10:27:11+0300</t>
         </is>
       </c>
       <c r="G98" t="b">
@@ -4835,36 +4831,36 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109564037</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110291970</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>Опыт работы с &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и Django. Знание принципов проектирования баз данных и опыт работы с. PostgreSQL. Опыт разработки RESTful API...</t>
+          <t>Высшее образование (Математическое/Информационные технологии). Понимание архитектуры данных. Опыт работы: с SQL, &lt;highlighttext&gt;Python&lt;/highlighttext&gt; (про часть работы с бд), Airflow, Superset...</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>Активами и интеграции с внешними финансовыми сервисами. Мы активно используем &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и Django для создания надежной и. Масштабируемой серверной архитектуры...</t>
+          <t>Анализ данных из систем-источников ( Postgres, greenplum). Построение отчетности на основе бизнес требований ( &lt;highlighttext&gt;Python&lt;/highlighttext&gt; , Airflow, superset ). Подготовка технической документации и...</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>109592349</t>
+          <t>110202463</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Python-разработчик (Junior)</t>
+          <t>Тестировщик — стажер в Сбер</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>71800</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4873,7 +4869,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2024-10-30T02:14:56+0300</t>
+          <t>2024-11-06T09:51:26+0300</t>
         </is>
       </c>
       <c r="G99" t="b">
@@ -4881,36 +4877,36 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109592349</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110202463</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Увлечен миром программирования и &lt;highlighttext&gt;Python&lt;/highlighttext&gt; - твой любимый язык, ты легко осваиваешь новые технологии и любишь решать сложные задачи. </t>
+          <t>Необходимые навыки: — Ansible. — Apache Kafka. — OpenShift. — REST API. — понимание микросервисной архитектуры.</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Разрабатывать backend-часть веб-приложений на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;: Ты будешь создавать логику приложения, разрабатывать API и интегрировать его с базами данных. </t>
+          <t xml:space="preserve">изучать характеристики нагрузочных тестов. — измерять параметры при запуске тестов и их влияние. — производить подготовку стенда перед запуском нагрузочного тестирования. — </t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>110130889</t>
+          <t>109420687</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Разработчик Python</t>
+          <t>Python-разработчик (Junior)</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>100000</v>
+        <v>75000</v>
       </c>
       <c r="D100" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -4919,7 +4915,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2024-11-05T14:30:36+0300</t>
+          <t>2024-11-08T11:17:36+0300</t>
         </is>
       </c>
       <c r="G100" t="b">
@@ -4927,36 +4923,36 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110130889</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109420687</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт коммерческой разработки от 1 года. Уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Git, Linux. Умение собирать и разворачивать проекты под ОС Linux. </t>
+          <t xml:space="preserve">Уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Опыт работы с FastAPI / Flask. Знание основ SQL. Опыт работы с Linux. Понимание основ работы с сетями. </t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>Разработка на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; скриптов. Работа с Raspberry. Работа с web socket. Разработка, организация и управление базами данных. Участие в разработке...</t>
+          <t>Разработкой API. Разработкой и реализацией Unit-тестов. Написанием технической документации.</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>110135402</t>
+          <t>109564037</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Python разработчик</t>
+          <t>Junior Backend-разработчик Django</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>180000</v>
+        <v>35000</v>
       </c>
       <c r="D101" t="n">
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -4965,7 +4961,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2024-11-05T15:21:38+0300</t>
+          <t>2024-11-07T15:56:31+0300</t>
         </is>
       </c>
       <c r="G101" t="b">
@@ -4973,43 +4969,45 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110135402</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109564037</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t xml:space="preserve">Коммерческий опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и использования Django / FastAPI от 3-х лет. Опыт работы с микросервисной архитектурой. </t>
+          <t>Опыт работы с &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и Django. Знание принципов проектирования баз данных и опыт работы с. PostgreSQL. Опыт разработки RESTful API...</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t xml:space="preserve">Участие в разработке проектов. Разработка backend (REST API ) для сервисов, как в рамках новых проектов, так и для уже существующих. </t>
+          <t>Активами и интеграции с внешними финансовыми сервисами. Мы активно используем &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и Django для создания надежной и. Масштабируемой серверной архитектуры...</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>110193554</t>
+          <t>109592349</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Senior QA инженер (мануальное тестирование)</t>
+          <t>Python-разработчик (Junior)</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
-      <c r="E102" t="n">
-        <v>0</v>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2024-11-06T07:29:23+0300</t>
+          <t>2024-10-30T02:14:56+0300</t>
         </is>
       </c>
       <c r="G102" t="b">
@@ -5017,43 +5015,45 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110193554</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109592349</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t xml:space="preserve">Понимание SDLC и потребностей разработки. Умение тестировать требования к ПО. Опыт исследовательского тестирования. Умение формировать чек-лист, предугадывать поведение системы. </t>
+          <t xml:space="preserve">Увлечен миром программирования и &lt;highlighttext&gt;Python&lt;/highlighttext&gt; - твой любимый язык, ты легко осваиваешь новые технологии и любишь решать сложные задачи. </t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Ручное функциональное, регрессионное, Smoke и приемочное тестирование Web приложений и Backend. Создание и актуализация тестовой документации: дизайн тест-кейсов, составление...</t>
+          <t xml:space="preserve">Разрабатывать backend-часть веб-приложений на &lt;highlighttext&gt;Python&lt;/highlighttext&gt;: Ты будешь создавать логику приложения, разрабатывать API и интегрировать его с базами данных. </t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>109052250</t>
+          <t>110130889</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Инженер по тестированию / QA Engineer</t>
+          <t>Разработчик Python</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
-      </c>
-      <c r="E103" t="n">
-        <v>0</v>
+        <v>200000</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2024-10-22T12:00:32+0300</t>
+          <t>2024-11-05T14:30:36+0300</t>
         </is>
       </c>
       <c r="G103" t="b">
@@ -5061,36 +5061,36 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=109052250</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110130889</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт работы с Docker\Postgresql\Etcd\Nginx\ProxmoxVE\Zabbix\AWX. Знание SQL. Хороший командный игрок. Базовые знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. </t>
+          <t xml:space="preserve">Опыт коммерческой разработки от 1 года. Уверенные знания &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, Git, Linux. Умение собирать и разворачивать проекты под ОС Linux. </t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Разработка тест-кейсов, чек-листов, оформление тест-планов. Выполнение ручного тестирования (desktop приложения). Мониторинг/поддержание в рабочем состоянии стендов тестирования. </t>
+          <t>Разработка на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; скриптов. Работа с Raspberry. Работа с web socket. Разработка, организация и управление базами данных. Участие в разработке...</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>110249813</t>
+          <t>110135402</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Web-разработчик</t>
+          <t>Python разработчик</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>50000</v>
+        <v>180000</v>
       </c>
       <c r="D104" t="n">
-        <v>50000</v>
+        <v>350000</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -5099,7 +5099,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2024-11-06T14:29:56+0300</t>
+          <t>2024-11-05T15:21:38+0300</t>
         </is>
       </c>
       <c r="G104" t="b">
@@ -5107,41 +5107,43 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110249813</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110135402</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>Знание Javascript, HTML, CSS - обязательно. VueJS, &lt;highlighttext&gt;Python&lt;/highlighttext&gt;, PHP, ArcGIS, QGIS, SQL - желательно.</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr"/>
+          <t xml:space="preserve">Коммерческий опыт разработки на &lt;highlighttext&gt;Python&lt;/highlighttext&gt; и использования Django / FastAPI от 3-х лет. Опыт работы с микросервисной архитектурой. </t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Участие в разработке проектов. Разработка backend (REST API ) для сервисов, как в рамках новых проектов, так и для уже существующих. </t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>110257193</t>
+          <t>110332560</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Аналитик геоданных</t>
+          <t>Python Backend Developer</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>130000</v>
+        <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>150000</v>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>RUR</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2024-11-06T16:12:05+0300</t>
+          <t>2024-11-07T16:38:24+0300</t>
         </is>
       </c>
       <c r="G105" t="b">
@@ -5149,17 +5151,17 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110257193</t>
+          <t>https://hh.ru/applicant/vacancy_response?vacancyId=110332560</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t xml:space="preserve">Высшее профессиональное образование в геологической сфере. Опыт работы в специализированных организациях от 3 лет. Владение специализированными программами (QGIS, ArcGIS). </t>
+          <t>Умение разбираться в чужом коде. Уверенное владение &lt;highlighttext&gt;Python&lt;/highlighttext&gt;. Понимание и умение писать асинхронный код. Опыт работы с Flask/FastAPI, SQLAlchemy...</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>Ведение базы данных показателей состояния подземных вод и опасных геологических процессов (PostgreSQL). Анализ данных мониторинга (статистический, пространственный) подземных вод и...</t>
+          <t>Разработка разных платформ. Проведения код-ревью. Рефакторинг, оптимизация и поддержка текущей кодовой базы. Оперативное решение проблем и устранение ошибок в...</t>
         </is>
       </c>
     </row>

</xml_diff>